<commit_message>
testcases and bug fix
</commit_message>
<xml_diff>
--- a/Menuitems.xlsx
+++ b/Menuitems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terre\Administrator\Desktop\CZ2002\oodpProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771DD95D-7019-42CC-A37E-15C51C117529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA5E5F7-3419-4BB9-A58A-557F52759580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{938EF673-AEEC-47AD-B6C8-BC98A229A5D5}"/>
   </bookViews>
@@ -105,18 +105,9 @@
     <t>Promotional set</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>Apple House's Steak comes with Mushroom soup and Lime juice</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>Classic Fish &amp; Chips</t>
   </si>
   <si>
@@ -145,6 +136,15 @@
   </si>
   <si>
     <t>floor(0.9*total original price)</t>
+  </si>
+  <si>
+    <t>ASet House's special</t>
+  </si>
+  <si>
+    <t>Set T-bone's special</t>
+  </si>
+  <si>
+    <t>Set Fishy meal</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -584,13 +584,13 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
       <c r="L2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -622,13 +622,13 @@
         <v>3.8</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -642,10 +642,10 @@
         <v>22.5</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -660,18 +660,18 @@
         <v>3.8</v>
       </c>
       <c r="J4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -680,19 +680,19 @@
         <v>15.5</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F5">
         <v>20</v>
       </c>
       <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
         <v>31</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
       </c>
       <c r="I5">
         <v>3</v>

</xml_diff>